<commit_message>
Change to 75% inclusion rule for COM.
</commit_message>
<xml_diff>
--- a/Data derived/COM slopes.xlsx
+++ b/Data derived/COM slopes.xlsx
@@ -15,12 +15,12 @@
     <sheet name="COM slopes" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="268">
   <si>
     <t>n</t>
   </si>
@@ -661,15 +661,9 @@
     <t>southern stingray</t>
   </si>
   <si>
-    <t>greenland halibut</t>
-  </si>
-  <si>
     <t>streamer bass</t>
   </si>
   <si>
-    <t>northern shrimp</t>
-  </si>
-  <si>
     <t>fourspot flounder</t>
   </si>
   <si>
@@ -694,15 +688,6 @@
     <t>gulf stream flounder</t>
   </si>
   <si>
-    <t>smooth skate</t>
-  </si>
-  <si>
-    <t>aesop shrimp</t>
-  </si>
-  <si>
-    <t>twospot flounder</t>
-  </si>
-  <si>
     <t>blue runner</t>
   </si>
   <si>
@@ -730,9 +715,6 @@
     <t>witch flounder</t>
   </si>
   <si>
-    <t>snow crab</t>
-  </si>
-  <si>
     <t>bigeye scad</t>
   </si>
   <si>
@@ -745,12 +727,6 @@
     <t>thorny skate</t>
   </si>
   <si>
-    <t>atlantic saury</t>
-  </si>
-  <si>
-    <t>pink glass shrimp</t>
-  </si>
-  <si>
     <t>round herring</t>
   </si>
   <si>
@@ -791,6 +767,63 @@
   </si>
   <si>
     <t>p-value</t>
+  </si>
+  <si>
+    <t>mostly on the shelf break</t>
+  </si>
+  <si>
+    <t>Possibility, but low sample size</t>
+  </si>
+  <si>
+    <t>possibility, but doesn't show up until Fall 1975 (survey issue?)</t>
+  </si>
+  <si>
+    <t>no; sample size too small</t>
+  </si>
+  <si>
+    <t>no; GOM fish</t>
+  </si>
+  <si>
+    <t>possibly; variable geographic distribution</t>
+  </si>
+  <si>
+    <t>located along shelf break</t>
+  </si>
+  <si>
+    <t>good canditate</t>
+  </si>
+  <si>
+    <t>Fish investigated for null modeling</t>
+  </si>
+  <si>
+    <t>Fish investigated in initial rounds</t>
+  </si>
+  <si>
+    <t>Fish here have been pre-filtered to include:</t>
+  </si>
+  <si>
+    <t>-only trawls after 1967</t>
+  </si>
+  <si>
+    <t>-only species that were caught off Delmarva at least once</t>
+  </si>
+  <si>
+    <t>Latitude slope</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>p&lt;0.001</t>
   </si>
 </sst>
 </file>
@@ -933,7 +966,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1119,6 +1152,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1280,17 +1319,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1633,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J489"/>
+  <dimension ref="A1:P421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A463" workbookViewId="0">
-      <selection activeCell="G295" sqref="G295"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,54 +1693,55 @@
     <col min="8" max="8" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E1" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E1" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -1724,10 +1767,13 @@
       <c r="J3" s="2">
         <v>0.247507251884203</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1753,8 +1799,11 @@
       <c r="J4" s="2">
         <v>5.4818006954134899E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M4" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>196</v>
       </c>
@@ -1782,8 +1831,11 @@
       <c r="J5" s="2">
         <v>0.91602747110348903</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M5" s="8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1812,7 +1864,7 @@
         <v>8.8628221687496401E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1840,9 +1892,12 @@
       <c r="J7" s="2">
         <v>0.90877233267353796</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="M7" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
@@ -1869,9 +1924,12 @@
       <c r="J8" s="2">
         <v>3.50108505446052E-6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="M8" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
@@ -1899,9 +1957,9 @@
         <v>1.30287448990675E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -1928,9 +1986,9 @@
         <v>0.18092340747160801</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -1956,8 +2014,11 @@
       <c r="J11" s="2">
         <v>9.7002084956356094E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1985,8 +2046,21 @@
       <c r="J12" s="2">
         <v>1.5695882045606201E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>263</v>
+      </c>
+      <c r="N12" s="1">
+        <f>MIN(E3:E421)</f>
+        <v>-22464.821624263401</v>
+      </c>
+      <c r="O12" t="s">
+        <v>266</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2014,8 +2088,18 @@
       <c r="J13" s="2">
         <v>0.20716646563647001</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>264</v>
+      </c>
+      <c r="N13" s="1">
+        <f>MEDIAN(E3:E421)</f>
+        <v>2278.69318510946</v>
+      </c>
+      <c r="P13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>205</v>
       </c>
@@ -2043,8 +2127,21 @@
       <c r="J14" s="2">
         <v>5.9902017145074399E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>265</v>
+      </c>
+      <c r="N14" s="1">
+        <f xml:space="preserve"> MAX(E3:E421)</f>
+        <v>15357.3631015347</v>
+      </c>
+      <c r="O14" t="s">
+        <v>267</v>
+      </c>
+      <c r="P14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>205</v>
       </c>
@@ -2073,9 +2170,9 @@
         <v>0.56653981211234905</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -2104,7 +2201,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -2394,7 +2491,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -2423,7 +2520,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
@@ -2451,7 +2548,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B29" t="s">
@@ -2480,7 +2577,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B30" t="s">
@@ -2626,7 +2723,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B35" t="s">
         <v>4</v>
@@ -2655,7 +2752,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -3061,7 +3158,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B50" t="s">
         <v>4</v>
@@ -3090,7 +3187,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
@@ -3931,7 +4028,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B80" t="s">
         <v>2</v>
@@ -4104,7 +4201,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B86" t="s">
@@ -4133,7 +4230,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B87" t="s">
@@ -4569,7 +4666,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B102" t="s">
         <v>2</v>
@@ -4771,7 +4868,7 @@
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B109" t="s">
@@ -4800,7 +4897,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
+      <c r="A110" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B110" t="s">
@@ -5350,7 +5447,7 @@
         <v>0.58900302721484799</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -5379,7 +5476,7 @@
         <v>0.32278601883814401</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>125</v>
       </c>
@@ -5408,7 +5505,7 @@
         <v>7.5385024827087393E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>125</v>
       </c>
@@ -5437,7 +5534,7 @@
         <v>0.60073997122470901</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>65</v>
       </c>
@@ -5466,7 +5563,7 @@
         <v>3.2554814471082001E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>65</v>
       </c>
@@ -5495,7 +5592,7 @@
         <v>5.7826128297514101E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -5524,7 +5621,7 @@
         <v>0.22854024855441901</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>201</v>
       </c>
@@ -5553,8 +5650,8 @@
         <v>0.53159530509311603</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B136" t="s">
@@ -5581,9 +5678,12 @@
       <c r="J136" s="2">
         <v>3.6549144013091799E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+      <c r="L136" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
         <v>165</v>
       </c>
       <c r="B137" t="s">
@@ -5610,8 +5710,11 @@
       <c r="J137" s="2">
         <v>0.388687855866447</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L137" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>147</v>
       </c>
@@ -5640,7 +5743,7 @@
         <v>3.1869897619595897E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>10</v>
       </c>
@@ -5669,7 +5772,7 @@
         <v>0.132105471338404</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>156</v>
       </c>
@@ -5698,7 +5801,7 @@
         <v>0.503203203059014</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>156</v>
       </c>
@@ -5727,7 +5830,7 @@
         <v>1.2849188190266899E-3</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>113</v>
       </c>
@@ -5756,7 +5859,7 @@
         <v>0.93444128865773801</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>113</v>
       </c>
@@ -5785,9 +5888,9 @@
         <v>0.19833060389191701</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B144" t="s">
         <v>4</v>
@@ -5814,9 +5917,9 @@
         <v>2.0068099774979899E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B145" t="s">
         <v>2</v>
@@ -5843,7 +5946,7 @@
         <v>4.8695356490431801E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>19</v>
       </c>
@@ -5872,7 +5975,7 @@
         <v>0.33942580455881499</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>19</v>
       </c>
@@ -5901,7 +6004,7 @@
         <v>7.4070222649027406E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>56</v>
       </c>
@@ -5930,7 +6033,7 @@
         <v>0.53650695588493102</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>56</v>
       </c>
@@ -5959,7 +6062,7 @@
         <v>0.73070823198998602</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>173</v>
       </c>
@@ -5988,7 +6091,7 @@
         <v>5.2741957905925903E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>111</v>
       </c>
@@ -6017,7 +6120,7 @@
         <v>0.76645663188090596</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>111</v>
       </c>
@@ -6046,7 +6149,7 @@
         <v>0.74849834456378805</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>54</v>
       </c>
@@ -6075,9 +6178,9 @@
         <v>0.77788829647786195</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>229</v>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A154" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="B154" t="s">
         <v>4</v>
@@ -6103,10 +6206,13 @@
       <c r="J154" s="2">
         <v>0.98625344032601703</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>229</v>
+      <c r="L154" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A155" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="B155" t="s">
         <v>2</v>
@@ -6132,8 +6238,11 @@
       <c r="J155" s="2">
         <v>7.6283967353469498E-2</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L155" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>67</v>
       </c>
@@ -6162,7 +6271,7 @@
         <v>1.54870534477666E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>63</v>
       </c>
@@ -6191,7 +6300,7 @@
         <v>0.26350573325918097</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>150</v>
       </c>
@@ -6220,7 +6329,7 @@
         <v>0.28802410701297998</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>150</v>
       </c>
@@ -6249,9 +6358,9 @@
         <v>5.1858382471605101E-6</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B160" t="s">
         <v>4</v>
@@ -6280,7 +6389,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B161" t="s">
         <v>2</v>
@@ -6628,7 +6737,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B173" t="s">
         <v>4</v>
@@ -6657,7 +6766,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B174" t="s">
         <v>2</v>
@@ -6742,7 +6851,7 @@
         <v>0.110578430111802</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>190</v>
       </c>
@@ -6771,7 +6880,7 @@
         <v>1.27155591447716E-4</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>190</v>
       </c>
@@ -6800,7 +6909,7 @@
         <v>1.5580934809581799E-7</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>33</v>
       </c>
@@ -6829,7 +6938,7 @@
         <v>6.6029379083064596E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>33</v>
       </c>
@@ -6858,7 +6967,7 @@
         <v>7.5879917364251703E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>172</v>
       </c>
@@ -6887,7 +6996,7 @@
         <v>0.112053781410671</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>172</v>
       </c>
@@ -6916,9 +7025,9 @@
         <v>5.1396308796798698E-3</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
-        <v>222</v>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A183" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="B183" t="s">
         <v>4</v>
@@ -6944,10 +7053,13 @@
       <c r="J183" s="2">
         <v>1.00585466452696E-2</v>
       </c>
-    </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
-        <v>222</v>
+      <c r="L183" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A184" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="B184" t="s">
         <v>2</v>
@@ -6973,8 +7085,11 @@
       <c r="J184" s="2">
         <v>2.1011387133055399E-2</v>
       </c>
-    </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L184" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>87</v>
       </c>
@@ -7003,7 +7118,7 @@
         <v>3.7150319684809197E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>87</v>
       </c>
@@ -7032,7 +7147,7 @@
         <v>0.65856890016511505</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>50</v>
       </c>
@@ -7061,7 +7176,7 @@
         <v>0.158502813162337</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>50</v>
       </c>
@@ -7090,7 +7205,7 @@
         <v>0.85409161306811998</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>61</v>
       </c>
@@ -7119,7 +7234,7 @@
         <v>1.2279849924895401E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>70</v>
       </c>
@@ -7148,7 +7263,7 @@
         <v>0.63564341520921297</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>70</v>
       </c>
@@ -7177,7 +7292,7 @@
         <v>9.5478288654761899E-7</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>103</v>
       </c>
@@ -7352,8 +7467,8 @@
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A198" s="5" t="s">
-        <v>230</v>
+      <c r="A198" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="B198" t="s">
         <v>4</v>
@@ -7381,8 +7496,8 @@
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A199" s="5" t="s">
-        <v>230</v>
+      <c r="A199" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="B199" t="s">
         <v>2</v>
@@ -7670,7 +7785,7 @@
         <v>3.1368664607832303E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>9</v>
       </c>
@@ -7699,9 +7814,9 @@
         <v>0.120019061449867</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A210" t="s">
-        <v>220</v>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A210" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="B210" t="s">
         <v>4</v>
@@ -7727,10 +7842,13 @@
       <c r="J210" s="2">
         <v>0.27411680745961903</v>
       </c>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
-        <v>220</v>
+      <c r="L210" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A211" s="6" t="s">
+        <v>218</v>
       </c>
       <c r="B211" t="s">
         <v>2</v>
@@ -7756,8 +7874,11 @@
       <c r="J211" s="2">
         <v>0.999459307085386</v>
       </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L211" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>109</v>
       </c>
@@ -7786,7 +7907,7 @@
         <v>0.80882346614859102</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>109</v>
       </c>
@@ -7815,7 +7936,7 @@
         <v>0.75263283499971101</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>158</v>
       </c>
@@ -7844,7 +7965,7 @@
         <v>0.95443060744906705</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>158</v>
       </c>
@@ -7873,7 +7994,7 @@
         <v>0.430987194033913</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>203</v>
       </c>
@@ -7902,8 +8023,8 @@
         <v>0.818933100337779</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A217" t="s">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A217" s="6" t="s">
         <v>209</v>
       </c>
       <c r="B217" t="s">
@@ -7930,9 +8051,12 @@
       <c r="J217" s="2">
         <v>9.4345747120355802E-2</v>
       </c>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
+      <c r="L217" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A218" s="6" t="s">
         <v>209</v>
       </c>
       <c r="B218" t="s">
@@ -7959,8 +8083,11 @@
       <c r="J218" s="2">
         <v>0.154926204164755</v>
       </c>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L218" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>3</v>
       </c>
@@ -7989,7 +8116,7 @@
         <v>0.500181216666853</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>3</v>
       </c>
@@ -8018,7 +8145,7 @@
         <v>0.588531702907234</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>95</v>
       </c>
@@ -8047,7 +8174,7 @@
         <v>5.5034355113651903E-4</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>95</v>
       </c>
@@ -8076,7 +8203,7 @@
         <v>0.15798935998467101</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>207</v>
       </c>
@@ -8105,7 +8232,7 @@
         <v>0.74705310196750596</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>207</v>
       </c>
@@ -8134,9 +8261,9 @@
         <v>0.59538699848382404</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B225" t="s">
         <v>4</v>
@@ -8163,9 +8290,9 @@
         <v>9.5157909797909196E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B226" t="s">
         <v>2</v>
@@ -8192,9 +8319,9 @@
         <v>8.7492724631562505E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A227" t="s">
-        <v>233</v>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A227" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="B227" t="s">
         <v>4</v>
@@ -8220,10 +8347,13 @@
       <c r="J227" s="2">
         <v>0.42867118618856798</v>
       </c>
-    </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A228" t="s">
-        <v>233</v>
+      <c r="L227" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A228" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="B228" t="s">
         <v>2</v>
@@ -8249,8 +8379,11 @@
       <c r="J228" s="2">
         <v>0.122650963459656</v>
       </c>
-    </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L228" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>140</v>
       </c>
@@ -8279,7 +8412,7 @@
         <v>9.0434392856834195E-4</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>140</v>
       </c>
@@ -8308,7 +8441,7 @@
         <v>8.1844905770324301E-7</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>82</v>
       </c>
@@ -8337,7 +8470,7 @@
         <v>0.112484553927445</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>82</v>
       </c>
@@ -8366,7 +8499,7 @@
         <v>2.83173729811209E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>152</v>
       </c>
@@ -8395,7 +8528,7 @@
         <v>0.66869091935776004</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>152</v>
       </c>
@@ -8424,7 +8557,7 @@
         <v>0.121222770590886</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>92</v>
       </c>
@@ -8453,7 +8586,7 @@
         <v>0.29032442476730402</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>92</v>
       </c>
@@ -8482,8 +8615,8 @@
         <v>0.65284334158835899</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A237" s="5" t="s">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A237" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B237" t="s">
@@ -8511,8 +8644,8 @@
         <v>0.75612472152343502</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A238" s="5" t="s">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A238" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B238" t="s">
@@ -8540,7 +8673,7 @@
         <v>0.60107550987985103</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>22</v>
       </c>
@@ -8569,7 +8702,7 @@
         <v>4.3366891154281599E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>133</v>
       </c>
@@ -8890,7 +9023,7 @@
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B251" t="s">
         <v>2</v>
@@ -9062,7 +9195,7 @@
         <v>7.1791954542269195E-4</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>68</v>
       </c>
@@ -9091,8 +9224,8 @@
         <v>1.5217840155103801E-3</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A258" t="s">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A258" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B258" t="s">
@@ -9119,9 +9252,12 @@
       <c r="J258" s="2">
         <v>3.1437788186270901E-4</v>
       </c>
-    </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A259" t="s">
+      <c r="L258" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A259" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B259" t="s">
@@ -9148,8 +9284,11 @@
       <c r="J259" s="2">
         <v>0.15563670891137399</v>
       </c>
-    </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L259" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>74</v>
       </c>
@@ -9178,9 +9317,9 @@
         <v>1.7197007023894501E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B261" t="s">
         <v>4</v>
@@ -9207,9 +9346,9 @@
         <v>3.7331191827086503E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B262" t="s">
         <v>2</v>
@@ -9236,7 +9375,7 @@
         <v>0.95500204938737099</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>153</v>
       </c>
@@ -9265,7 +9404,7 @@
         <v>0.190733754729602</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>153</v>
       </c>
@@ -9294,7 +9433,7 @@
         <v>0.439663394240565</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>84</v>
       </c>
@@ -9323,7 +9462,7 @@
         <v>0.50156508098125296</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>84</v>
       </c>
@@ -9352,7 +9491,7 @@
         <v>0.97470817447818503</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>187</v>
       </c>
@@ -9381,7 +9520,7 @@
         <v>3.9125371926473501E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>187</v>
       </c>
@@ -9410,7 +9549,7 @@
         <v>0.471316180824428</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>83</v>
       </c>
@@ -9439,7 +9578,7 @@
         <v>8.9521941121553997E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>29</v>
       </c>
@@ -9468,7 +9607,7 @@
         <v>8.5033001142650597E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>36</v>
       </c>
@@ -9497,8 +9636,8 @@
         <v>0.44716783955394002</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A272" s="5" t="s">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A272" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B272" t="s">
@@ -9527,7 +9666,7 @@
       </c>
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A273" s="5" t="s">
+      <c r="A273" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B273" t="s">
@@ -10021,7 +10160,7 @@
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B290" t="s">
         <v>4</v>
@@ -10050,7 +10189,7 @@
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B291" t="s">
         <v>2</v>
@@ -10079,7 +10218,7 @@
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B292" t="s">
         <v>4</v>
@@ -10108,7 +10247,7 @@
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B293" t="s">
         <v>2</v>
@@ -10339,7 +10478,7 @@
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A301" s="5" t="s">
+      <c r="A301" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B301" t="s">
@@ -10368,7 +10507,7 @@
       </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A302" s="5" t="s">
+      <c r="A302" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B302" t="s">
@@ -10454,7 +10593,7 @@
         <v>0.14769170294707301</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>210</v>
       </c>
@@ -10483,7 +10622,7 @@
         <v>1.03748900757546E-2</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>139</v>
       </c>
@@ -10512,7 +10651,7 @@
         <v>0.44584871704915602</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>139</v>
       </c>
@@ -10541,7 +10680,7 @@
         <v>0.136486438063393</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>11</v>
       </c>
@@ -10570,7 +10709,7 @@
         <v>5.0348549365083102E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>18</v>
       </c>
@@ -10599,7 +10738,7 @@
         <v>0.67323747386289901</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>18</v>
       </c>
@@ -10628,7 +10767,7 @@
         <v>0.59143878228364399</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>99</v>
       </c>
@@ -10657,7 +10796,7 @@
         <v>0.84712220606350497</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>99</v>
       </c>
@@ -10686,7 +10825,7 @@
         <v>0.93221919557227995</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>96</v>
       </c>
@@ -10715,7 +10854,7 @@
         <v>0.62335942916068898</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>96</v>
       </c>
@@ -10744,8 +10883,8 @@
         <v>0.27396017261198702</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A315" t="s">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A315" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B315" t="s">
@@ -10772,9 +10911,12 @@
       <c r="J315" s="2">
         <v>0.28726903947329602</v>
       </c>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A316" t="s">
+      <c r="L315" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A316" s="6" t="s">
         <v>177</v>
       </c>
       <c r="B316" t="s">
@@ -10801,8 +10943,11 @@
       <c r="J316" s="2">
         <v>0.76526759461354199</v>
       </c>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L316" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>13</v>
       </c>
@@ -10831,7 +10976,7 @@
         <v>0.39366828997792802</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>13</v>
       </c>
@@ -10860,7 +11005,7 @@
         <v>6.46992871158513E-3</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>48</v>
       </c>
@@ -10889,8 +11034,8 @@
         <v>0.48195735322664501</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A320" s="5" t="s">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A320" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B320" t="s">
@@ -10918,8 +11063,8 @@
         <v>0.63426672914734705</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A321" s="5" t="s">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A321" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B321" t="s">
@@ -10947,7 +11092,7 @@
         <v>4.3621936963749197E-5</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>148</v>
       </c>
@@ -10976,7 +11121,7 @@
         <v>0.71118073246797098</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>51</v>
       </c>
@@ -11005,7 +11150,7 @@
         <v>7.9821897300792699E-2</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>49</v>
       </c>
@@ -11034,7 +11179,7 @@
         <v>4.4781861528132699E-5</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>49</v>
       </c>
@@ -11063,7 +11208,7 @@
         <v>2.4616324976960298E-3</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>171</v>
       </c>
@@ -11092,7 +11237,7 @@
         <v>0.20853742721670601</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>171</v>
       </c>
@@ -11121,7 +11266,7 @@
         <v>0.71274167701979596</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>31</v>
       </c>
@@ -11150,7 +11295,7 @@
         <v>3.5576366785933498E-3</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>14</v>
       </c>
@@ -11179,7 +11324,7 @@
         <v>0.25616048738877101</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>15</v>
       </c>
@@ -11208,7 +11353,7 @@
         <v>0.13549619213639799</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>102</v>
       </c>
@@ -11237,7 +11382,7 @@
         <v>0.54723707283990997</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>102</v>
       </c>
@@ -11266,8 +11411,8 @@
         <v>0.82307873610858995</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A333" t="s">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A333" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B333" t="s">
@@ -11294,9 +11439,12 @@
       <c r="J333" s="2">
         <v>0.94508664968498102</v>
       </c>
-    </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A334" t="s">
+      <c r="L333" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A334" s="6" t="s">
         <v>179</v>
       </c>
       <c r="B334" t="s">
@@ -11323,8 +11471,11 @@
       <c r="J334" s="2">
         <v>0.97272865695769395</v>
       </c>
-    </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L334" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>182</v>
       </c>
@@ -11353,7 +11504,7 @@
         <v>0.58686106319586595</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>182</v>
       </c>
@@ -11383,7 +11534,7 @@
       </c>
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A337" s="5" t="s">
+      <c r="A337" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B337" t="s">
@@ -11412,7 +11563,7 @@
       </c>
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A338" s="5" t="s">
+      <c r="A338" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B338" t="s">
@@ -11529,7 +11680,7 @@
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B342" t="s">
         <v>4</v>
@@ -11558,7 +11709,7 @@
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B343" t="s">
         <v>2</v>
@@ -12282,7 +12433,7 @@
       </c>
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A368" s="5" t="s">
+      <c r="A368" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B368" t="s">
@@ -12311,7 +12462,7 @@
       </c>
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A369" s="5" t="s">
+      <c r="A369" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B369" t="s">
@@ -12428,7 +12579,7 @@
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B373" t="s">
         <v>4</v>
@@ -12457,7 +12608,7 @@
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B374" t="s">
         <v>2</v>
@@ -12660,7 +12811,7 @@
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B381" t="s">
         <v>2</v>
@@ -12804,7 +12955,7 @@
       </c>
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A386" s="5" t="s">
+      <c r="A386" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B386" t="s">
@@ -12833,7 +12984,7 @@
       </c>
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A387" s="5" t="s">
+      <c r="A387" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B387" t="s">
@@ -12921,7 +13072,7 @@
     </row>
     <row r="390" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B390" t="s">
         <v>4</v>
@@ -12950,7 +13101,7 @@
     </row>
     <row r="391" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B391" t="s">
         <v>2</v>
@@ -13037,7 +13188,7 @@
     </row>
     <row r="394" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B394" t="s">
         <v>2</v>
@@ -13066,7 +13217,7 @@
     </row>
     <row r="395" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B395" t="s">
         <v>4</v>
@@ -13095,7 +13246,7 @@
     </row>
     <row r="396" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B396" t="s">
         <v>2</v>
@@ -13210,7 +13361,7 @@
       </c>
     </row>
     <row r="400" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A400" s="5" t="s">
+      <c r="A400" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B400" t="s">
@@ -13239,7 +13390,7 @@
       </c>
     </row>
     <row r="401" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A401" s="5" t="s">
+      <c r="A401" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B401" t="s">
@@ -13356,7 +13507,7 @@
     </row>
     <row r="405" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B405" t="s">
         <v>4</v>
@@ -13558,7 +13709,7 @@
       </c>
     </row>
     <row r="412" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A412" s="5" t="s">
+      <c r="A412" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B412" t="s">
@@ -13587,7 +13738,7 @@
       </c>
     </row>
     <row r="413" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A413" s="5" t="s">
+      <c r="A413" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B413" t="s">
@@ -13617,7 +13768,7 @@
     </row>
     <row r="414" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B414" t="s">
         <v>4</v>
@@ -13646,7 +13797,7 @@
     </row>
     <row r="415" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B415" t="s">
         <v>2</v>
@@ -13845,1978 +13996,6 @@
       </c>
       <c r="J421" s="2">
         <v>0.64869957750456697</v>
-      </c>
-    </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A422" t="s">
-        <v>212</v>
-      </c>
-      <c r="B422" t="s">
-        <v>2</v>
-      </c>
-      <c r="C422">
-        <v>36</v>
-      </c>
-      <c r="E422" s="1">
-        <v>1171.75156483623</v>
-      </c>
-      <c r="F422" s="2">
-        <v>0.30514501443495101</v>
-      </c>
-      <c r="G422" s="1">
-        <v>761.41013665573701</v>
-      </c>
-      <c r="H422" s="2">
-        <v>0.23532853757289601</v>
-      </c>
-      <c r="I422" s="2">
-        <v>-2.75197063706039E-2</v>
-      </c>
-      <c r="J422" s="2">
-        <v>0.70376023514195596</v>
-      </c>
-    </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A423" t="s">
-        <v>212</v>
-      </c>
-      <c r="B423" t="s">
-        <v>4</v>
-      </c>
-      <c r="C423">
-        <v>20</v>
-      </c>
-      <c r="E423" s="1">
-        <v>-1153.95892787651</v>
-      </c>
-      <c r="F423" s="2">
-        <v>0.21678987264119101</v>
-      </c>
-      <c r="G423" s="1">
-        <v>814.69661811645506</v>
-      </c>
-      <c r="H423" s="2">
-        <v>0.10130229412416999</v>
-      </c>
-      <c r="I423" s="2">
-        <v>0.16703882024750699</v>
-      </c>
-      <c r="J423" s="2">
-        <v>0.69112494305832695</v>
-      </c>
-    </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A424" t="s">
-        <v>213</v>
-      </c>
-      <c r="B424" t="s">
-        <v>2</v>
-      </c>
-      <c r="C424">
-        <v>15</v>
-      </c>
-      <c r="E424" s="1">
-        <v>1162.48697344891</v>
-      </c>
-      <c r="F424" s="2">
-        <v>0.72928889733269797</v>
-      </c>
-      <c r="G424" s="1">
-        <v>182.329457318533</v>
-      </c>
-      <c r="H424" s="2">
-        <v>0.96095535098006202</v>
-      </c>
-      <c r="I424" s="2">
-        <v>-0.42161066048648799</v>
-      </c>
-      <c r="J424" s="2">
-        <v>0.89876388322536704</v>
-      </c>
-    </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A425" t="s">
-        <v>213</v>
-      </c>
-      <c r="B425" t="s">
-        <v>4</v>
-      </c>
-      <c r="C425">
-        <v>18</v>
-      </c>
-      <c r="E425" s="1">
-        <v>-553.43632180046995</v>
-      </c>
-      <c r="F425" s="2">
-        <v>0.73882764918180799</v>
-      </c>
-      <c r="G425" s="1">
-        <v>-7369.0806167602104</v>
-      </c>
-      <c r="H425" s="2">
-        <v>1.4677259992768E-4</v>
-      </c>
-      <c r="I425" s="2">
-        <v>-1.3691425468518501</v>
-      </c>
-      <c r="J425" s="2">
-        <v>0.13471967996141601</v>
-      </c>
-    </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A426" t="s">
-        <v>214</v>
-      </c>
-      <c r="B426" t="s">
-        <v>4</v>
-      </c>
-      <c r="C426">
-        <v>20</v>
-      </c>
-      <c r="E426" s="1">
-        <v>1154.8727819020701</v>
-      </c>
-      <c r="F426" s="2">
-        <v>0.57594940057911004</v>
-      </c>
-      <c r="G426" s="1">
-        <v>1703.5111613101001</v>
-      </c>
-      <c r="H426" s="2">
-        <v>0.37629421755881098</v>
-      </c>
-      <c r="I426" s="2">
-        <v>0.35991688457642501</v>
-      </c>
-      <c r="J426" s="2">
-        <v>0.69101710328789001</v>
-      </c>
-    </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A427" t="s">
-        <v>214</v>
-      </c>
-      <c r="B427" t="s">
-        <v>2</v>
-      </c>
-      <c r="C427">
-        <v>12</v>
-      </c>
-      <c r="E427" s="1">
-        <v>119.579012618568</v>
-      </c>
-      <c r="F427" s="2">
-        <v>0.81915890355759902</v>
-      </c>
-      <c r="G427" s="1">
-        <v>203.04092404345801</v>
-      </c>
-      <c r="H427" s="2">
-        <v>0.64660552676638094</v>
-      </c>
-      <c r="I427" s="2">
-        <v>0.63819152092419895</v>
-      </c>
-      <c r="J427" s="2">
-        <v>0.35962403604460003</v>
-      </c>
-    </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A428" t="s">
-        <v>215</v>
-      </c>
-      <c r="B428" t="s">
-        <v>2</v>
-      </c>
-      <c r="C428">
-        <v>39</v>
-      </c>
-      <c r="E428" s="1">
-        <v>1116.1084517593599</v>
-      </c>
-      <c r="F428" s="2">
-        <v>1.38864454225774E-5</v>
-      </c>
-      <c r="G428" s="1">
-        <v>-74.864387033768693</v>
-      </c>
-      <c r="H428" s="2">
-        <v>0.82207992282147802</v>
-      </c>
-      <c r="I428" s="2">
-        <v>-0.26070196346798302</v>
-      </c>
-      <c r="J428" s="2">
-        <v>0.26194336603388102</v>
-      </c>
-    </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A429" t="s">
-        <v>215</v>
-      </c>
-      <c r="B429" t="s">
-        <v>4</v>
-      </c>
-      <c r="C429">
-        <v>31</v>
-      </c>
-      <c r="E429" s="1">
-        <v>664.07049523182104</v>
-      </c>
-      <c r="F429" s="2">
-        <v>2.39758681692126E-2</v>
-      </c>
-      <c r="G429" s="1">
-        <v>57.271894712788303</v>
-      </c>
-      <c r="H429" s="2">
-        <v>0.87567859780044399</v>
-      </c>
-      <c r="I429" s="2">
-        <v>-0.124659533740222</v>
-      </c>
-      <c r="J429" s="2">
-        <v>0.44152518547067199</v>
-      </c>
-    </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A430" t="s">
-        <v>216</v>
-      </c>
-      <c r="B430" t="s">
-        <v>2</v>
-      </c>
-      <c r="C430">
-        <v>53</v>
-      </c>
-      <c r="E430" s="1">
-        <v>1112.1651211457399</v>
-      </c>
-      <c r="F430" s="2">
-        <v>4.4161488216033001E-3</v>
-      </c>
-      <c r="G430" s="1">
-        <v>2481.24685081386</v>
-      </c>
-      <c r="H430" s="2">
-        <v>8.63577901654203E-7</v>
-      </c>
-      <c r="I430" s="2">
-        <v>0.58250625535186396</v>
-      </c>
-      <c r="J430" s="2">
-        <v>3.7557156508097399E-8</v>
-      </c>
-    </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A431" t="s">
-        <v>216</v>
-      </c>
-      <c r="B431" t="s">
-        <v>4</v>
-      </c>
-      <c r="C431">
-        <v>52</v>
-      </c>
-      <c r="E431" s="1">
-        <v>177.11073808706701</v>
-      </c>
-      <c r="F431" s="2">
-        <v>0.51314159522814196</v>
-      </c>
-      <c r="G431" s="1">
-        <v>1420.6578426501101</v>
-      </c>
-      <c r="H431" s="2">
-        <v>1.33622317371893E-3</v>
-      </c>
-      <c r="I431" s="2">
-        <v>0.64701149135601699</v>
-      </c>
-      <c r="J431" s="2">
-        <v>2.3880898825604401E-5</v>
-      </c>
-    </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A432" t="s">
-        <v>217</v>
-      </c>
-      <c r="B432" t="s">
-        <v>4</v>
-      </c>
-      <c r="C432">
-        <v>11</v>
-      </c>
-      <c r="E432" s="1">
-        <v>-1100.2291644535701</v>
-      </c>
-      <c r="F432" s="2">
-        <v>0.75700419699769494</v>
-      </c>
-      <c r="G432" s="1">
-        <v>-1625.4929984231101</v>
-      </c>
-      <c r="H432" s="2">
-        <v>0.72307384746269998</v>
-      </c>
-      <c r="I432" s="2">
-        <v>0.59079399311561198</v>
-      </c>
-      <c r="J432" s="2">
-        <v>0.264755269476317</v>
-      </c>
-    </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A433" t="s">
-        <v>218</v>
-      </c>
-      <c r="B433" t="s">
-        <v>4</v>
-      </c>
-      <c r="C433">
-        <v>32</v>
-      </c>
-      <c r="E433" s="1">
-        <v>1096.7201750208201</v>
-      </c>
-      <c r="F433" s="2">
-        <v>1.8803387623090799E-2</v>
-      </c>
-      <c r="G433" s="1">
-        <v>1223.8004407619201</v>
-      </c>
-      <c r="H433" s="2">
-        <v>7.8972523005675904E-3</v>
-      </c>
-      <c r="I433" s="2">
-        <v>0.185312607923068</v>
-      </c>
-      <c r="J433" s="2">
-        <v>0.46904755713634</v>
-      </c>
-    </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A434" t="s">
-        <v>218</v>
-      </c>
-      <c r="B434" t="s">
-        <v>2</v>
-      </c>
-      <c r="C434">
-        <v>41</v>
-      </c>
-      <c r="E434" s="1">
-        <v>838.27452783509204</v>
-      </c>
-      <c r="F434" s="2">
-        <v>0.46719734383908001</v>
-      </c>
-      <c r="G434" s="1">
-        <v>2437.8582972535601</v>
-      </c>
-      <c r="H434" s="2">
-        <v>3.7717675025730199E-4</v>
-      </c>
-      <c r="I434" s="2">
-        <v>0.42852961241761101</v>
-      </c>
-      <c r="J434" s="2">
-        <v>1.52842725105887E-2</v>
-      </c>
-    </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A435" t="s">
-        <v>219</v>
-      </c>
-      <c r="B435" t="s">
-        <v>2</v>
-      </c>
-      <c r="C435">
-        <v>50</v>
-      </c>
-      <c r="E435" s="1">
-        <v>1094.4384391886799</v>
-      </c>
-      <c r="F435" s="2">
-        <v>0.59389871906999703</v>
-      </c>
-      <c r="G435" s="1">
-        <v>2954.3563928612798</v>
-      </c>
-      <c r="H435" s="2">
-        <v>5.13100193082308E-2</v>
-      </c>
-      <c r="I435" s="2">
-        <v>0.373115854063578</v>
-      </c>
-      <c r="J435" s="2">
-        <v>2.8736775601755801E-2</v>
-      </c>
-    </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A436" t="s">
-        <v>219</v>
-      </c>
-      <c r="B436" t="s">
-        <v>4</v>
-      </c>
-      <c r="C436">
-        <v>24</v>
-      </c>
-      <c r="E436" s="1">
-        <v>611.07086182553905</v>
-      </c>
-      <c r="F436" s="2">
-        <v>0.65430217942778701</v>
-      </c>
-      <c r="G436" s="1">
-        <v>1791.0598047748399</v>
-      </c>
-      <c r="H436" s="2">
-        <v>0.106401144892307</v>
-      </c>
-      <c r="I436" s="2">
-        <v>-0.16234879948463099</v>
-      </c>
-      <c r="J436" s="2">
-        <v>0.54885080259246</v>
-      </c>
-    </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A437" t="s">
-        <v>220</v>
-      </c>
-      <c r="B437" t="s">
-        <v>2</v>
-      </c>
-      <c r="C437">
-        <v>32</v>
-      </c>
-      <c r="E437" s="1">
-        <v>1061.45140680247</v>
-      </c>
-      <c r="F437" s="2">
-        <v>0.65676429321109897</v>
-      </c>
-      <c r="G437" s="1">
-        <v>2596.8200047154</v>
-      </c>
-      <c r="H437" s="2">
-        <v>0.28288451244391999</v>
-      </c>
-      <c r="I437" s="2">
-        <v>5.85317192777318E-4</v>
-      </c>
-      <c r="J437" s="2">
-        <v>0.999459307085386</v>
-      </c>
-    </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A438" t="s">
-        <v>220</v>
-      </c>
-      <c r="B438" t="s">
-        <v>4</v>
-      </c>
-      <c r="C438">
-        <v>31</v>
-      </c>
-      <c r="E438" s="1">
-        <v>-135.38858792262101</v>
-      </c>
-      <c r="F438" s="2">
-        <v>0.96145982504844496</v>
-      </c>
-      <c r="G438" s="1">
-        <v>251.620910577074</v>
-      </c>
-      <c r="H438" s="2">
-        <v>0.930924348786071</v>
-      </c>
-      <c r="I438" s="2">
-        <v>0.93559776755708801</v>
-      </c>
-      <c r="J438" s="2">
-        <v>0.27411680745961903</v>
-      </c>
-    </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A439" t="s">
-        <v>221</v>
-      </c>
-      <c r="B439" t="s">
-        <v>4</v>
-      </c>
-      <c r="C439">
-        <v>52</v>
-      </c>
-      <c r="E439" s="1">
-        <v>-1042.9537057131799</v>
-      </c>
-      <c r="F439" s="2">
-        <v>6.0391532210546999E-6</v>
-      </c>
-      <c r="G439" s="1">
-        <v>474.42999431425102</v>
-      </c>
-      <c r="H439" s="2">
-        <v>0.18143962802003799</v>
-      </c>
-      <c r="I439" s="2">
-        <v>0.30168212534924299</v>
-      </c>
-      <c r="J439" s="2">
-        <v>2.0068099774979899E-2</v>
-      </c>
-    </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A440" t="s">
-        <v>221</v>
-      </c>
-      <c r="B440" t="s">
-        <v>2</v>
-      </c>
-      <c r="C440">
-        <v>53</v>
-      </c>
-      <c r="E440" s="1">
-        <v>-392.90794779441302</v>
-      </c>
-      <c r="F440" s="2">
-        <v>5.73374648720417E-2</v>
-      </c>
-      <c r="G440" s="1">
-        <v>267.29631436906101</v>
-      </c>
-      <c r="H440" s="2">
-        <v>0.41640123161341402</v>
-      </c>
-      <c r="I440" s="2">
-        <v>0.38225767460751497</v>
-      </c>
-      <c r="J440" s="2">
-        <v>4.8695356490431801E-2</v>
-      </c>
-    </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A441" t="s">
-        <v>222</v>
-      </c>
-      <c r="B441" t="s">
-        <v>4</v>
-      </c>
-      <c r="C441">
-        <v>44</v>
-      </c>
-      <c r="E441" s="1">
-        <v>-1039.37789256876</v>
-      </c>
-      <c r="F441" s="2">
-        <v>0.24124605149310399</v>
-      </c>
-      <c r="G441" s="1">
-        <v>103.0316974956</v>
-      </c>
-      <c r="H441" s="2">
-        <v>0.62727859765947902</v>
-      </c>
-      <c r="I441" s="2">
-        <v>0.600413507371232</v>
-      </c>
-      <c r="J441" s="2">
-        <v>1.00585466452696E-2</v>
-      </c>
-    </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A442" t="s">
-        <v>222</v>
-      </c>
-      <c r="B442" t="s">
-        <v>2</v>
-      </c>
-      <c r="C442">
-        <v>45</v>
-      </c>
-      <c r="E442" s="1">
-        <v>870.229167189701</v>
-      </c>
-      <c r="F442" s="2">
-        <v>0.210378392339541</v>
-      </c>
-      <c r="G442" s="1">
-        <v>343.19826703852101</v>
-      </c>
-      <c r="H442" s="2">
-        <v>4.5998685670492298E-2</v>
-      </c>
-      <c r="I442" s="2">
-        <v>0.29954502231026398</v>
-      </c>
-      <c r="J442" s="2">
-        <v>2.1011387133055399E-2</v>
-      </c>
-    </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A443" t="s">
-        <v>223</v>
-      </c>
-      <c r="B443" t="s">
-        <v>2</v>
-      </c>
-      <c r="C443">
-        <v>53</v>
-      </c>
-      <c r="E443" s="1">
-        <v>1032.49462873375</v>
-      </c>
-      <c r="F443" s="2">
-        <v>7.5043939043827806E-2</v>
-      </c>
-      <c r="G443" s="1">
-        <v>343.30539361864601</v>
-      </c>
-      <c r="H443" s="2">
-        <v>0.64651933289359598</v>
-      </c>
-      <c r="I443" s="2">
-        <v>-0.24404850836028699</v>
-      </c>
-      <c r="J443" s="2">
-        <v>0.27426439199404301</v>
-      </c>
-    </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A444" t="s">
-        <v>223</v>
-      </c>
-      <c r="B444" t="s">
-        <v>4</v>
-      </c>
-      <c r="C444">
-        <v>52</v>
-      </c>
-      <c r="E444" s="1">
-        <v>357.13148422457698</v>
-      </c>
-      <c r="F444" s="2">
-        <v>0.56141053945348796</v>
-      </c>
-      <c r="G444" s="1">
-        <v>-341.17640799965301</v>
-      </c>
-      <c r="H444" s="2">
-        <v>0.65319944758741</v>
-      </c>
-      <c r="I444" s="2">
-        <v>-5.99716395564115E-2</v>
-      </c>
-      <c r="J444" s="2">
-        <v>0.75946922462984801</v>
-      </c>
-    </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A445" t="s">
-        <v>224</v>
-      </c>
-      <c r="B445" t="s">
-        <v>4</v>
-      </c>
-      <c r="C445">
-        <v>52</v>
-      </c>
-      <c r="E445" s="1">
-        <v>993.37315931292596</v>
-      </c>
-      <c r="F445" s="2">
-        <v>2.6092975559852201E-3</v>
-      </c>
-      <c r="G445" s="1">
-        <v>582.35723077032105</v>
-      </c>
-      <c r="H445" s="2">
-        <v>4.3549863140594502E-2</v>
-      </c>
-      <c r="I445" s="2">
-        <v>0.52572337052061302</v>
-      </c>
-      <c r="J445" s="2">
-        <v>6.9218136680432299E-3</v>
-      </c>
-    </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A446" t="s">
-        <v>224</v>
-      </c>
-      <c r="B446" t="s">
-        <v>2</v>
-      </c>
-      <c r="C446">
-        <v>53</v>
-      </c>
-      <c r="E446" s="1">
-        <v>576.277302666987</v>
-      </c>
-      <c r="F446" s="2">
-        <v>5.3346831552433797E-2</v>
-      </c>
-      <c r="G446" s="1">
-        <v>-351.32121283463101</v>
-      </c>
-      <c r="H446" s="2">
-        <v>0.25543964700166799</v>
-      </c>
-      <c r="I446" s="2">
-        <v>0.40752351529177899</v>
-      </c>
-      <c r="J446" s="2">
-        <v>3.0664310532159799E-2</v>
-      </c>
-    </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A447" t="s">
-        <v>225</v>
-      </c>
-      <c r="B447" t="s">
-        <v>2</v>
-      </c>
-      <c r="C447">
-        <v>28</v>
-      </c>
-      <c r="E447" s="1">
-        <v>-960.49558579269501</v>
-      </c>
-      <c r="F447" s="2">
-        <v>0.39377449804313902</v>
-      </c>
-      <c r="G447" s="1">
-        <v>1119.27350985931</v>
-      </c>
-      <c r="H447" s="2">
-        <v>0.4976561817506</v>
-      </c>
-      <c r="I447" s="2">
-        <v>1.12723454559096</v>
-      </c>
-      <c r="J447" s="2">
-        <v>2.0711119451878101E-2</v>
-      </c>
-    </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A448" t="s">
-        <v>225</v>
-      </c>
-      <c r="B448" t="s">
-        <v>4</v>
-      </c>
-      <c r="C448">
-        <v>22</v>
-      </c>
-      <c r="E448" s="1">
-        <v>622.58412597225004</v>
-      </c>
-      <c r="F448" s="2">
-        <v>0.42849807053232503</v>
-      </c>
-      <c r="G448" s="1">
-        <v>1580.4250452787401</v>
-      </c>
-      <c r="H448" s="2">
-        <v>9.3896340558117297E-2</v>
-      </c>
-      <c r="I448" s="2">
-        <v>-0.12588756288522099</v>
-      </c>
-      <c r="J448" s="2">
-        <v>0.722988753020681</v>
-      </c>
-    </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A449" t="s">
-        <v>226</v>
-      </c>
-      <c r="B449" t="s">
-        <v>2</v>
-      </c>
-      <c r="C449">
-        <v>13</v>
-      </c>
-      <c r="E449" s="1">
-        <v>908.38101617054394</v>
-      </c>
-      <c r="F449" s="2">
-        <v>0.14422738640685101</v>
-      </c>
-      <c r="G449" s="1">
-        <v>2077.0560084857202</v>
-      </c>
-      <c r="H449" s="2">
-        <v>8.12664323374373E-2</v>
-      </c>
-      <c r="I449" s="2">
-        <v>1.3755135320506999</v>
-      </c>
-      <c r="J449" s="2">
-        <v>8.1961795637557804E-4</v>
-      </c>
-    </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A450" t="s">
-        <v>227</v>
-      </c>
-      <c r="B450" t="s">
-        <v>2</v>
-      </c>
-      <c r="C450">
-        <v>48</v>
-      </c>
-      <c r="E450" s="1">
-        <v>896.96875522116102</v>
-      </c>
-      <c r="F450" s="2">
-        <v>0.52610718872136397</v>
-      </c>
-      <c r="G450" s="1">
-        <v>1163.5853944477999</v>
-      </c>
-      <c r="H450" s="2">
-        <v>0.249383876535861</v>
-      </c>
-      <c r="I450" s="2">
-        <v>-0.49755030375502801</v>
-      </c>
-      <c r="J450" s="2">
-        <v>0.392385975555823</v>
-      </c>
-    </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A451" t="s">
-        <v>228</v>
-      </c>
-      <c r="B451" t="s">
-        <v>2</v>
-      </c>
-      <c r="C451">
-        <v>39</v>
-      </c>
-      <c r="E451" s="1">
-        <v>872.26330913579898</v>
-      </c>
-      <c r="F451" s="2">
-        <v>0.65821266912609599</v>
-      </c>
-      <c r="G451" s="1">
-        <v>954.41051304672203</v>
-      </c>
-      <c r="H451" s="2">
-        <v>0.27795661366770902</v>
-      </c>
-      <c r="I451" s="2">
-        <v>0.24293670455292099</v>
-      </c>
-      <c r="J451" s="2">
-        <v>2.5476850397841401E-4</v>
-      </c>
-    </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A452" t="s">
-        <v>229</v>
-      </c>
-      <c r="B452" t="s">
-        <v>4</v>
-      </c>
-      <c r="C452">
-        <v>52</v>
-      </c>
-      <c r="E452" s="1">
-        <v>796.88367384030403</v>
-      </c>
-      <c r="F452" s="2">
-        <v>0.190944811775169</v>
-      </c>
-      <c r="G452" s="1">
-        <v>1215.84550389529</v>
-      </c>
-      <c r="H452" s="2">
-        <v>0.112954403690537</v>
-      </c>
-      <c r="I452" s="2">
-        <v>4.7638829916308396E-3</v>
-      </c>
-      <c r="J452" s="2">
-        <v>0.98625344032601703</v>
-      </c>
-    </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A453" t="s">
-        <v>229</v>
-      </c>
-      <c r="B453" t="s">
-        <v>2</v>
-      </c>
-      <c r="C453">
-        <v>53</v>
-      </c>
-      <c r="E453" s="1">
-        <v>615.37248348788796</v>
-      </c>
-      <c r="F453" s="2">
-        <v>0.24138512280323399</v>
-      </c>
-      <c r="G453" s="1">
-        <v>1360.48124449483</v>
-      </c>
-      <c r="H453" s="2">
-        <v>7.7418517591200303E-2</v>
-      </c>
-      <c r="I453" s="2">
-        <v>0.34234453176525798</v>
-      </c>
-      <c r="J453" s="2">
-        <v>7.6283967353469498E-2</v>
-      </c>
-    </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A454" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B454" t="s">
-        <v>4</v>
-      </c>
-      <c r="C454">
-        <v>52</v>
-      </c>
-      <c r="E454" s="1">
-        <v>-745.017858734431</v>
-      </c>
-      <c r="F454" s="2">
-        <v>3.4936984949492998E-3</v>
-      </c>
-      <c r="G454" s="1">
-        <v>-1980.4408783480401</v>
-      </c>
-      <c r="H454" s="2">
-        <v>8.3754176318342199E-3</v>
-      </c>
-      <c r="I454" s="2">
-        <v>-0.189776874568164</v>
-      </c>
-      <c r="J454" s="2">
-        <v>0.119746393851745</v>
-      </c>
-    </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A455" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B455" t="s">
-        <v>2</v>
-      </c>
-      <c r="C455">
-        <v>53</v>
-      </c>
-      <c r="E455" s="1">
-        <v>-510.03943467130199</v>
-      </c>
-      <c r="F455" s="2">
-        <v>1.6209839640995701E-2</v>
-      </c>
-      <c r="G455" s="1">
-        <v>-1469.1857028450099</v>
-      </c>
-      <c r="H455" s="2">
-        <v>2.2796101348077798E-2</v>
-      </c>
-      <c r="I455" s="2">
-        <v>-6.2708210740911499E-2</v>
-      </c>
-      <c r="J455" s="2">
-        <v>0.41108960307102699</v>
-      </c>
-    </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A456" t="s">
-        <v>231</v>
-      </c>
-      <c r="B456" t="s">
-        <v>4</v>
-      </c>
-      <c r="C456">
-        <v>52</v>
-      </c>
-      <c r="E456" s="1">
-        <v>714.35459741529996</v>
-      </c>
-      <c r="F456" s="2">
-        <v>2.8331764557950102E-2</v>
-      </c>
-      <c r="G456" s="1">
-        <v>-2193.8880910009102</v>
-      </c>
-      <c r="H456" s="2">
-        <v>1.5809886038013301E-3</v>
-      </c>
-      <c r="I456" s="2">
-        <v>0.60777151933977802</v>
-      </c>
-      <c r="J456" s="2">
-        <v>3.7331191827086503E-2</v>
-      </c>
-    </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A457" t="s">
-        <v>231</v>
-      </c>
-      <c r="B457" t="s">
-        <v>2</v>
-      </c>
-      <c r="C457">
-        <v>53</v>
-      </c>
-      <c r="E457" s="1">
-        <v>533.94771969549299</v>
-      </c>
-      <c r="F457" s="2">
-        <v>8.9572773524177002E-2</v>
-      </c>
-      <c r="G457" s="1">
-        <v>-936.15172748535497</v>
-      </c>
-      <c r="H457" s="2">
-        <v>0.158890617859375</v>
-      </c>
-      <c r="I457" s="2">
-        <v>1.51622900602233E-2</v>
-      </c>
-      <c r="J457" s="2">
-        <v>0.95500204938737099</v>
-      </c>
-    </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A458" t="s">
-        <v>232</v>
-      </c>
-      <c r="B458" t="s">
-        <v>2</v>
-      </c>
-      <c r="C458">
-        <v>24</v>
-      </c>
-      <c r="E458" s="1">
-        <v>-699.35907084975202</v>
-      </c>
-      <c r="F458" s="2">
-        <v>0.83135669119751798</v>
-      </c>
-      <c r="G458" s="1">
-        <v>-2654.1539245232598</v>
-      </c>
-      <c r="H458" s="2">
-        <v>0.44931184094830101</v>
-      </c>
-      <c r="I458" s="2">
-        <v>-0.99902520158988795</v>
-      </c>
-      <c r="J458" s="2">
-        <v>8.7492724631562505E-2</v>
-      </c>
-    </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A459" t="s">
-        <v>232</v>
-      </c>
-      <c r="B459" t="s">
-        <v>4</v>
-      </c>
-      <c r="C459">
-        <v>21</v>
-      </c>
-      <c r="E459" s="1">
-        <v>133.98067018563</v>
-      </c>
-      <c r="F459" s="2">
-        <v>0.96601484668068804</v>
-      </c>
-      <c r="G459" s="1">
-        <v>-1206.21020352956</v>
-      </c>
-      <c r="H459" s="2">
-        <v>0.726757700842246</v>
-      </c>
-      <c r="I459" s="2">
-        <v>-0.96856772218244602</v>
-      </c>
-      <c r="J459" s="2">
-        <v>9.5157909797909196E-2</v>
-      </c>
-    </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A460" t="s">
-        <v>233</v>
-      </c>
-      <c r="B460" t="s">
-        <v>4</v>
-      </c>
-      <c r="C460">
-        <v>48</v>
-      </c>
-      <c r="E460" s="1">
-        <v>-637.859332728921</v>
-      </c>
-      <c r="F460" s="2">
-        <v>0.22816440371610899</v>
-      </c>
-      <c r="G460" s="1">
-        <v>27.627218278856802</v>
-      </c>
-      <c r="H460" s="2">
-        <v>0.96715409895646198</v>
-      </c>
-      <c r="I460" s="2">
-        <v>0.120075843412377</v>
-      </c>
-      <c r="J460" s="2">
-        <v>0.42867118618856798</v>
-      </c>
-    </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A461" t="s">
-        <v>233</v>
-      </c>
-      <c r="B461" t="s">
-        <v>2</v>
-      </c>
-      <c r="C461">
-        <v>51</v>
-      </c>
-      <c r="E461" s="1">
-        <v>-541.74903148388398</v>
-      </c>
-      <c r="F461" s="2">
-        <v>0.21352097370588399</v>
-      </c>
-      <c r="G461" s="1">
-        <v>-1212.0102468914199</v>
-      </c>
-      <c r="H461" s="2">
-        <v>1.6022025992122699E-2</v>
-      </c>
-      <c r="I461" s="2">
-        <v>0.47858051444438499</v>
-      </c>
-      <c r="J461" s="2">
-        <v>0.122650963459656</v>
-      </c>
-    </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A462" t="s">
-        <v>234</v>
-      </c>
-      <c r="B462" t="s">
-        <v>2</v>
-      </c>
-      <c r="C462">
-        <v>53</v>
-      </c>
-      <c r="E462" s="1">
-        <v>-615.75952274740996</v>
-      </c>
-      <c r="F462" s="2">
-        <v>1.87661881928093E-3</v>
-      </c>
-      <c r="G462" s="1">
-        <v>-2200.4671213974402</v>
-      </c>
-      <c r="H462" s="2">
-        <v>1.62208108191551E-5</v>
-      </c>
-      <c r="I462" s="2">
-        <v>0.23952185425688399</v>
-      </c>
-      <c r="J462" s="2">
-        <v>5.4818006954134899E-2</v>
-      </c>
-    </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A463" t="s">
-        <v>234</v>
-      </c>
-      <c r="B463" t="s">
-        <v>4</v>
-      </c>
-      <c r="C463">
-        <v>52</v>
-      </c>
-      <c r="E463" s="1">
-        <v>-69.062330946586201</v>
-      </c>
-      <c r="F463" s="2">
-        <v>0.80882648617720299</v>
-      </c>
-      <c r="G463" s="1">
-        <v>-1376.6573217681901</v>
-      </c>
-      <c r="H463" s="2">
-        <v>1.29401092303312E-2</v>
-      </c>
-      <c r="I463" s="2">
-        <v>-0.16089848834621301</v>
-      </c>
-      <c r="J463" s="2">
-        <v>0.247507251884203</v>
-      </c>
-    </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A464" t="s">
-        <v>235</v>
-      </c>
-      <c r="B464" t="s">
-        <v>4</v>
-      </c>
-      <c r="C464">
-        <v>52</v>
-      </c>
-      <c r="E464" s="1">
-        <v>-595.26948942090701</v>
-      </c>
-      <c r="F464" s="2">
-        <v>0.35412278100259198</v>
-      </c>
-      <c r="G464" s="1">
-        <v>-383.80813601564103</v>
-      </c>
-      <c r="H464" s="2">
-        <v>0.40052670872841201</v>
-      </c>
-      <c r="I464" s="2">
-        <v>0.61863365701786999</v>
-      </c>
-      <c r="J464" s="2">
-        <v>1.6105806404226701E-3</v>
-      </c>
-    </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A465" t="s">
-        <v>235</v>
-      </c>
-      <c r="B465" t="s">
-        <v>2</v>
-      </c>
-      <c r="C465">
-        <v>53</v>
-      </c>
-      <c r="E465" s="1">
-        <v>157.848434303896</v>
-      </c>
-      <c r="F465" s="2">
-        <v>0.67324775645563295</v>
-      </c>
-      <c r="G465" s="1">
-        <v>-178.13796713810299</v>
-      </c>
-      <c r="H465" s="2">
-        <v>0.62034091474721698</v>
-      </c>
-      <c r="I465" s="2">
-        <v>0.62178190046720805</v>
-      </c>
-      <c r="J465" s="2">
-        <v>2.13172764609959E-5</v>
-      </c>
-    </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A466" t="s">
-        <v>236</v>
-      </c>
-      <c r="B466" t="s">
-        <v>4</v>
-      </c>
-      <c r="C466">
-        <v>29</v>
-      </c>
-      <c r="E466" s="1">
-        <v>592.453082528962</v>
-      </c>
-      <c r="F466" s="2">
-        <v>0.37469586207287497</v>
-      </c>
-      <c r="G466" s="1">
-        <v>-1703.83611186191</v>
-      </c>
-      <c r="H466" s="2">
-        <v>0.128416983191113</v>
-      </c>
-      <c r="I466" s="2">
-        <v>-1.37104515319404</v>
-      </c>
-      <c r="J466" s="2">
-        <v>5.4852306061031898E-2</v>
-      </c>
-    </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A467" t="s">
-        <v>236</v>
-      </c>
-      <c r="B467" t="s">
-        <v>2</v>
-      </c>
-      <c r="C467">
-        <v>24</v>
-      </c>
-      <c r="E467" s="1">
-        <v>68.961813141942599</v>
-      </c>
-      <c r="F467" s="2">
-        <v>0.95141808863339905</v>
-      </c>
-      <c r="G467" s="1">
-        <v>-2194.3247448859602</v>
-      </c>
-      <c r="H467" s="2">
-        <v>9.4052780283151796E-2</v>
-      </c>
-      <c r="I467" s="2">
-        <v>-5.3389167135596903E-2</v>
-      </c>
-      <c r="J467" s="2">
-        <v>0.93251869012894795</v>
-      </c>
-    </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A468" t="s">
-        <v>237</v>
-      </c>
-      <c r="B468" t="s">
-        <v>2</v>
-      </c>
-      <c r="C468">
-        <v>48</v>
-      </c>
-      <c r="E468" s="1">
-        <v>-544.44415896895305</v>
-      </c>
-      <c r="F468" s="2">
-        <v>0.74514264336262004</v>
-      </c>
-      <c r="G468" s="1">
-        <v>473.64080607471197</v>
-      </c>
-      <c r="H468" s="2">
-        <v>0.67301508395642495</v>
-      </c>
-      <c r="I468" s="2">
-        <v>0.12565709947408299</v>
-      </c>
-      <c r="J468" s="2">
-        <v>0.23198437709755099</v>
-      </c>
-    </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A469" t="s">
-        <v>238</v>
-      </c>
-      <c r="B469" t="s">
-        <v>4</v>
-      </c>
-      <c r="C469">
-        <v>52</v>
-      </c>
-      <c r="E469" s="1">
-        <v>475.466428748184</v>
-      </c>
-      <c r="F469" s="2">
-        <v>0.48036941505636799</v>
-      </c>
-      <c r="G469" s="1">
-        <v>268.74581517880898</v>
-      </c>
-      <c r="H469" s="2">
-        <v>0.74095940651471204</v>
-      </c>
-      <c r="I469" s="2">
-        <v>0.25093671119493</v>
-      </c>
-      <c r="J469" s="2">
-        <v>3.4658821776318301E-2</v>
-      </c>
-    </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A470" t="s">
-        <v>238</v>
-      </c>
-      <c r="B470" t="s">
-        <v>2</v>
-      </c>
-      <c r="C470">
-        <v>53</v>
-      </c>
-      <c r="E470" s="1">
-        <v>373.419100401604</v>
-      </c>
-      <c r="F470" s="2">
-        <v>0.36187628918317299</v>
-      </c>
-      <c r="G470" s="1">
-        <v>-396.83152811148</v>
-      </c>
-      <c r="H470" s="2">
-        <v>0.44866691784106699</v>
-      </c>
-      <c r="I470" s="2">
-        <v>0.27594706995933599</v>
-      </c>
-      <c r="J470" s="2">
-        <v>0.28652883254888201</v>
-      </c>
-    </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A471" t="s">
-        <v>239</v>
-      </c>
-      <c r="B471" t="s">
-        <v>2</v>
-      </c>
-      <c r="C471">
-        <v>43</v>
-      </c>
-      <c r="E471" s="1">
-        <v>-462.60660393188101</v>
-      </c>
-      <c r="F471" s="2">
-        <v>0.59886093950159702</v>
-      </c>
-      <c r="G471" s="1">
-        <v>410.11144332162797</v>
-      </c>
-      <c r="H471" s="2">
-        <v>0.604845329387519</v>
-      </c>
-      <c r="I471" s="2">
-        <v>0.49818974986905501</v>
-      </c>
-      <c r="J471" s="2">
-        <v>0.22689684481057901</v>
-      </c>
-    </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A472" t="s">
-        <v>239</v>
-      </c>
-      <c r="B472" t="s">
-        <v>4</v>
-      </c>
-      <c r="C472">
-        <v>48</v>
-      </c>
-      <c r="E472" s="1">
-        <v>106.905321102009</v>
-      </c>
-      <c r="F472" s="2">
-        <v>0.87593429623742702</v>
-      </c>
-      <c r="G472" s="1">
-        <v>487.68840003276398</v>
-      </c>
-      <c r="H472" s="2">
-        <v>0.59893006047224095</v>
-      </c>
-      <c r="I472" s="2">
-        <v>0.422874902629928</v>
-      </c>
-      <c r="J472" s="2">
-        <v>0.19519120351569</v>
-      </c>
-    </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A473" t="s">
-        <v>240</v>
-      </c>
-      <c r="B473" t="s">
-        <v>4</v>
-      </c>
-      <c r="C473">
-        <v>52</v>
-      </c>
-      <c r="E473" s="1">
-        <v>-430.33501794948501</v>
-      </c>
-      <c r="F473" s="2">
-        <v>8.1950803227405E-2</v>
-      </c>
-      <c r="G473" s="1">
-        <v>-1878.9779944193299</v>
-      </c>
-      <c r="H473" s="2">
-        <v>1.4097622638476501E-6</v>
-      </c>
-      <c r="I473" s="2">
-        <v>-0.45833806018691797</v>
-      </c>
-      <c r="J473" s="2">
-        <v>2.9492269152305399E-3</v>
-      </c>
-    </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A474" t="s">
-        <v>240</v>
-      </c>
-      <c r="B474" t="s">
-        <v>2</v>
-      </c>
-      <c r="C474">
-        <v>53</v>
-      </c>
-      <c r="E474" s="1">
-        <v>-406.26697290741902</v>
-      </c>
-      <c r="F474" s="2">
-        <v>0.129518568741021</v>
-      </c>
-      <c r="G474" s="1">
-        <v>-1561.49235547739</v>
-      </c>
-      <c r="H474" s="2">
-        <v>9.3487364836065297E-5</v>
-      </c>
-      <c r="I474" s="2">
-        <v>-0.32060117786720699</v>
-      </c>
-      <c r="J474" s="2">
-        <v>2.9403332581029399E-2</v>
-      </c>
-    </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A475" t="s">
-        <v>241</v>
-      </c>
-      <c r="B475" t="s">
-        <v>2</v>
-      </c>
-      <c r="C475">
-        <v>47</v>
-      </c>
-      <c r="E475" s="1">
-        <v>-328.29600634064002</v>
-      </c>
-      <c r="F475" s="2">
-        <v>0.633963706049537</v>
-      </c>
-      <c r="G475" s="1">
-        <v>-2265.1007443251601</v>
-      </c>
-      <c r="H475" s="2">
-        <v>8.9797276200901202E-4</v>
-      </c>
-      <c r="I475" s="2">
-        <v>0.306994131638398</v>
-      </c>
-      <c r="J475" s="2">
-        <v>0.58717510562473596</v>
-      </c>
-    </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A476" t="s">
-        <v>242</v>
-      </c>
-      <c r="B476" t="s">
-        <v>4</v>
-      </c>
-      <c r="C476">
-        <v>22</v>
-      </c>
-      <c r="E476" s="1">
-        <v>-325.84342019101899</v>
-      </c>
-      <c r="F476" s="2">
-        <v>0.78059187933531204</v>
-      </c>
-      <c r="G476" s="1">
-        <v>1280.2014245785399</v>
-      </c>
-      <c r="H476" s="2">
-        <v>0.213765133282796</v>
-      </c>
-      <c r="I476" s="2">
-        <v>1.0932793839178001</v>
-      </c>
-      <c r="J476" s="2">
-        <v>0.15764012254298701</v>
-      </c>
-    </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A477" t="s">
-        <v>242</v>
-      </c>
-      <c r="B477" t="s">
-        <v>2</v>
-      </c>
-      <c r="C477">
-        <v>28</v>
-      </c>
-      <c r="E477" s="1">
-        <v>-55.294648357263803</v>
-      </c>
-      <c r="F477" s="2">
-        <v>0.96104482124464896</v>
-      </c>
-      <c r="G477" s="1">
-        <v>-551.882142559145</v>
-      </c>
-      <c r="H477" s="2">
-        <v>0.67545517711643599</v>
-      </c>
-      <c r="I477" s="2">
-        <v>0.23002519787096801</v>
-      </c>
-      <c r="J477" s="2">
-        <v>0.63210605266306297</v>
-      </c>
-    </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A478" t="s">
-        <v>243</v>
-      </c>
-      <c r="B478" t="s">
-        <v>2</v>
-      </c>
-      <c r="C478">
-        <v>52</v>
-      </c>
-      <c r="E478" s="1">
-        <v>-308.25241925872001</v>
-      </c>
-      <c r="F478" s="2">
-        <v>0.839111827895066</v>
-      </c>
-      <c r="G478" s="1">
-        <v>-184.79679311103601</v>
-      </c>
-      <c r="H478" s="2">
-        <v>0.846308361245659</v>
-      </c>
-      <c r="I478" s="2">
-        <v>-0.23415674240689699</v>
-      </c>
-      <c r="J478" s="2">
-        <v>0.24045358789042601</v>
-      </c>
-    </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A479" t="s">
-        <v>243</v>
-      </c>
-      <c r="B479" t="s">
-        <v>4</v>
-      </c>
-      <c r="C479">
-        <v>32</v>
-      </c>
-      <c r="E479" s="1">
-        <v>74.569797667086306</v>
-      </c>
-      <c r="F479" s="2">
-        <v>0.94283854445875204</v>
-      </c>
-      <c r="G479" s="1">
-        <v>1577.8938999172999</v>
-      </c>
-      <c r="H479" s="2">
-        <v>8.6098967479801003E-2</v>
-      </c>
-      <c r="I479" s="2">
-        <v>1.3199815879113701</v>
-      </c>
-      <c r="J479" s="2">
-        <v>0.10122323202532101</v>
-      </c>
-    </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A480" t="s">
-        <v>244</v>
-      </c>
-      <c r="B480" t="s">
-        <v>4</v>
-      </c>
-      <c r="C480">
-        <v>35</v>
-      </c>
-      <c r="E480" s="1">
-        <v>271.34132465383601</v>
-      </c>
-      <c r="F480" s="2">
-        <v>0.75286104505673501</v>
-      </c>
-      <c r="G480" s="1">
-        <v>-580.88314931325601</v>
-      </c>
-      <c r="H480" s="2">
-        <v>0.52516323412459298</v>
-      </c>
-      <c r="I480" s="2">
-        <v>-0.62641542217867097</v>
-      </c>
-      <c r="J480" s="2">
-        <v>2.5918970294615401E-2</v>
-      </c>
-    </row>
-    <row r="481" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A481" t="s">
-        <v>244</v>
-      </c>
-      <c r="B481" t="s">
-        <v>2</v>
-      </c>
-      <c r="C481">
-        <v>29</v>
-      </c>
-      <c r="E481" s="1">
-        <v>-89.598084553843606</v>
-      </c>
-      <c r="F481" s="2">
-        <v>0.905902957477979</v>
-      </c>
-      <c r="G481" s="1">
-        <v>-696.66380331709399</v>
-      </c>
-      <c r="H481" s="2">
-        <v>0.51610000266070399</v>
-      </c>
-      <c r="I481" s="2">
-        <v>-0.65888664895078997</v>
-      </c>
-      <c r="J481" s="2">
-        <v>0.308617935864404</v>
-      </c>
-    </row>
-    <row r="482" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A482" t="s">
-        <v>245</v>
-      </c>
-      <c r="B482" t="s">
-        <v>4</v>
-      </c>
-      <c r="C482">
-        <v>52</v>
-      </c>
-      <c r="E482" s="1">
-        <v>268.05750213418901</v>
-      </c>
-      <c r="F482" s="2">
-        <v>9.7169305084297206E-2</v>
-      </c>
-      <c r="G482" s="1">
-        <v>-1812.4636987143299</v>
-      </c>
-      <c r="H482" s="2">
-        <v>3.2203308760252701E-4</v>
-      </c>
-      <c r="I482" s="2">
-        <v>-0.28913943856543001</v>
-      </c>
-      <c r="J482" s="2">
-        <v>5.5396313932076703E-2</v>
-      </c>
-    </row>
-    <row r="483" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A483" t="s">
-        <v>245</v>
-      </c>
-      <c r="B483" t="s">
-        <v>2</v>
-      </c>
-      <c r="C483">
-        <v>53</v>
-      </c>
-      <c r="E483" s="1">
-        <v>-165.22260698758799</v>
-      </c>
-      <c r="F483" s="2">
-        <v>0.35712215832175498</v>
-      </c>
-      <c r="G483" s="1">
-        <v>-1577.2405826525201</v>
-      </c>
-      <c r="H483" s="2">
-        <v>2.60675776277753E-4</v>
-      </c>
-      <c r="I483" s="2">
-        <v>-0.32530383689164899</v>
-      </c>
-      <c r="J483" s="2">
-        <v>8.5519938186804593E-3</v>
-      </c>
-    </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A484" t="s">
-        <v>246</v>
-      </c>
-      <c r="B484" t="s">
-        <v>4</v>
-      </c>
-      <c r="C484">
-        <v>50</v>
-      </c>
-      <c r="E484" s="1">
-        <v>250.91311420916301</v>
-      </c>
-      <c r="F484" s="2">
-        <v>0.60399499491687902</v>
-      </c>
-      <c r="G484" s="1">
-        <v>313.40240615080802</v>
-      </c>
-      <c r="H484" s="2">
-        <v>0.24259804228804399</v>
-      </c>
-      <c r="I484" s="2">
-        <v>0.769979562524015</v>
-      </c>
-      <c r="J484" s="2">
-        <v>7.0981670051731199E-2</v>
-      </c>
-    </row>
-    <row r="485" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A485" t="s">
-        <v>246</v>
-      </c>
-      <c r="B485" t="s">
-        <v>2</v>
-      </c>
-      <c r="C485">
-        <v>52</v>
-      </c>
-      <c r="E485" s="1">
-        <v>143.657724344244</v>
-      </c>
-      <c r="F485" s="2">
-        <v>0.80030689981864001</v>
-      </c>
-      <c r="G485" s="1">
-        <v>191.13212110094901</v>
-      </c>
-      <c r="H485" s="2">
-        <v>0.16731653414179901</v>
-      </c>
-      <c r="I485" s="2">
-        <v>0.29194960220723098</v>
-      </c>
-      <c r="J485" s="2">
-        <v>3.3917161487035299E-3</v>
-      </c>
-    </row>
-    <row r="486" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A486" t="s">
-        <v>247</v>
-      </c>
-      <c r="B486" t="s">
-        <v>2</v>
-      </c>
-      <c r="C486">
-        <v>12</v>
-      </c>
-      <c r="E486" s="1">
-        <v>-114.565917376683</v>
-      </c>
-      <c r="F486" s="2">
-        <v>0.98510080252264498</v>
-      </c>
-      <c r="G486" s="1">
-        <v>2290.0458651112099</v>
-      </c>
-      <c r="H486" s="2">
-        <v>0.482308513273358</v>
-      </c>
-      <c r="I486" s="2">
-        <v>0.50751278772382902</v>
-      </c>
-      <c r="J486" s="2">
-        <v>1.90676713727402E-3</v>
-      </c>
-    </row>
-    <row r="487" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A487" t="s">
-        <v>248</v>
-      </c>
-      <c r="B487" t="s">
-        <v>4</v>
-      </c>
-      <c r="C487">
-        <v>52</v>
-      </c>
-      <c r="E487" s="1">
-        <v>-91.558489907478105</v>
-      </c>
-      <c r="F487" s="2">
-        <v>0.515138211896771</v>
-      </c>
-      <c r="G487" s="1">
-        <v>-2454.4287523818898</v>
-      </c>
-      <c r="H487" s="2">
-        <v>1.3472617534134901E-10</v>
-      </c>
-      <c r="I487" s="2">
-        <v>-0.16647976661115199</v>
-      </c>
-      <c r="J487" s="2">
-        <v>0.18092340747160801</v>
-      </c>
-    </row>
-    <row r="488" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A488" t="s">
-        <v>248</v>
-      </c>
-      <c r="B488" t="s">
-        <v>2</v>
-      </c>
-      <c r="C488">
-        <v>53</v>
-      </c>
-      <c r="E488" s="1">
-        <v>25.2140276084188</v>
-      </c>
-      <c r="F488" s="2">
-        <v>0.85820245850799703</v>
-      </c>
-      <c r="G488" s="1">
-        <v>-1684.1431448871001</v>
-      </c>
-      <c r="H488" s="2">
-        <v>3.3603282672166998E-6</v>
-      </c>
-      <c r="I488" s="2">
-        <v>0.23016080575182701</v>
-      </c>
-      <c r="J488" s="2">
-        <v>9.7002084956356094E-2</v>
-      </c>
-    </row>
-    <row r="489" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A489" t="s">
-        <v>249</v>
-      </c>
-      <c r="B489" t="s">
-        <v>2</v>
-      </c>
-      <c r="C489">
-        <v>24</v>
-      </c>
-      <c r="E489" s="1">
-        <v>-43.302053380567699</v>
-      </c>
-      <c r="F489" s="2">
-        <v>0.99239878095972001</v>
-      </c>
-      <c r="G489" s="1">
-        <v>3109.8749953552401</v>
-      </c>
-      <c r="H489" s="2">
-        <v>0.213563349715606</v>
-      </c>
-      <c r="I489" s="2">
-        <v>0.80897845149673997</v>
-      </c>
-      <c r="J489" s="2">
-        <v>3.1413878988238803E-2</v>
       </c>
     </row>
   </sheetData>
@@ -15825,12 +14004,12 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2 H2 J2">
+  <conditionalFormatting sqref="F2 H2 J2 M7">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J489 H3:H489 F3:F489">
+  <conditionalFormatting sqref="J3:J421 H3:H421 F3:F421">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>

</xml_diff>